<commit_message>
Updated transp files/adjust aircraft
</commit_message>
<xml_diff>
--- a/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
+++ b/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
@@ -2224,7 +2224,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -2364,7 +2364,6 @@
         </is>
       </c>
     </row>
-    <row r="24"/>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId1"/>
@@ -71694,7 +71693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:G6"/>

</xml_diff>